<commit_message>
Tests passing, Dereferencer stable.
</commit_message>
<xml_diff>
--- a/src/test/resources/poiji_datasets/test_dataset.xlsx
+++ b/src/test/resources/poiji_datasets/test_dataset.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="22980" windowHeight="9555"/>
   </bookViews>
   <sheets>
     <sheet name="rdf-dereferencer" sheetId="1" r:id="rId1"/>
@@ -888,14 +888,14 @@
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -921,22 +921,22 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>58</v>
@@ -944,46 +944,46 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4" t="s">
-        <v>160</v>
+      <c r="A7" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1671,12 +1671,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="B5" r:id="rId6"/>
+    <hyperlink ref="B6" r:id="rId7"/>
     <hyperlink ref="B9" r:id="rId8"/>
     <hyperlink ref="B11" r:id="rId9" location="type" display="http://www.w3.org/1999/02/22-rdf-syntax-ns - type"/>
     <hyperlink ref="B12" r:id="rId10" location="rest" display="http://www.w3.org/1999/02/22-rdf-syntax-ns - rest"/>
@@ -1752,7 +1752,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -1820,7 +1820,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New class AppConfig incorporated in tests and the next part of the project. Faulty tests for catching labels for WOT and foaf:mbox.
</commit_message>
<xml_diff>
--- a/src/test/resources/poiji_datasets/test_dataset.xlsx
+++ b/src/test/resources/poiji_datasets/test_dataset.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="167">
   <si>
     <t>testName</t>
   </si>
@@ -211,9 +211,6 @@
     <t>Dublin Core Metadata Element Set, Version 1.1</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>The OWL 2 Schema vocabulary (OWL 2)</t>
   </si>
   <si>
@@ -524,6 +521,21 @@
   </si>
   <si>
     <t>DC Elements</t>
+  </si>
+  <si>
+    <t>rdf-schema</t>
+  </si>
+  <si>
+    <t>skos.rdf</t>
+  </si>
+  <si>
+    <t>index.rdf</t>
+  </si>
+  <si>
+    <t>Q42</t>
+  </si>
+  <si>
+    <t>about.rdf</t>
   </si>
 </sst>
 </file>
@@ -887,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D8"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -903,7 +915,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -917,51 +929,51 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -977,18 +989,18 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
@@ -999,7 +1011,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -1010,7 +1022,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>16</v>
@@ -1021,7 +1033,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>18</v>
@@ -1032,7 +1044,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -1043,7 +1055,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>19</v>
@@ -1054,7 +1066,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>20</v>
@@ -1065,7 +1077,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>21</v>
@@ -1076,7 +1088,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>22</v>
@@ -1087,7 +1099,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>29</v>
@@ -1098,7 +1110,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>30</v>
@@ -1109,7 +1121,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>31</v>
@@ -1120,7 +1132,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>32</v>
@@ -1131,7 +1143,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>33</v>
@@ -1142,7 +1154,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>34</v>
@@ -1153,7 +1165,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>35</v>
@@ -1164,7 +1176,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>36</v>
@@ -1175,7 +1187,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>11</v>
@@ -1186,7 +1198,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>37</v>
@@ -1197,7 +1209,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>38</v>
@@ -1208,7 +1220,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>39</v>
@@ -1219,7 +1231,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>40</v>
@@ -1230,7 +1242,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>41</v>
@@ -1241,7 +1253,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>42</v>
@@ -1252,230 +1264,230 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="C48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="C50" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" t="s">
         <v>137</v>
-      </c>
-      <c r="C52" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C53" t="s">
         <v>14</v>
@@ -1483,10 +1495,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C54" t="s">
         <v>51</v>
@@ -1494,10 +1506,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C55" t="s">
         <v>52</v>
@@ -1505,10 +1517,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C56" t="s">
         <v>53</v>
@@ -1516,156 +1528,156 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C58" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C59" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C62" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C63" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C64" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="C65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C66" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C67" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1759,54 +1771,54 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
         <v>146</v>
       </c>
-      <c r="B4" t="s">
-        <v>147</v>
-      </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed dataset for faulty WOT and mbox. Some test classes need checking after the update to the new AppConfig and removal of ConfigurationManager.
</commit_message>
<xml_diff>
--- a/src/test/resources/poiji_datasets/test_dataset.xlsx
+++ b/src/test/resources/poiji_datasets/test_dataset.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="175">
   <si>
     <t>testName</t>
   </si>
@@ -536,6 +536,30 @@
   </si>
   <si>
     <t>about.rdf</t>
+  </si>
+  <si>
+    <t>hasKey</t>
+  </si>
+  <si>
+    <t>pubkeyAddress</t>
+  </si>
+  <si>
+    <t>fingerprint</t>
+  </si>
+  <si>
+    <t>identity</t>
+  </si>
+  <si>
+    <t>assurance</t>
+  </si>
+  <si>
+    <t>signed</t>
+  </si>
+  <si>
+    <t>signer</t>
+  </si>
+  <si>
+    <t>mbox</t>
   </si>
 </sst>
 </file>
@@ -897,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1262,7 +1286,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -1270,10 +1294,13 @@
         <v>60</v>
       </c>
       <c r="C33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -1281,10 +1308,13 @@
         <v>61</v>
       </c>
       <c r="C34" t="s">
+        <v>168</v>
+      </c>
+      <c r="D34" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -1292,10 +1322,13 @@
         <v>62</v>
       </c>
       <c r="C35" t="s">
+        <v>169</v>
+      </c>
+      <c r="D35" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -1303,10 +1336,13 @@
         <v>63</v>
       </c>
       <c r="C36" t="s">
+        <v>170</v>
+      </c>
+      <c r="D36" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -1314,10 +1350,13 @@
         <v>64</v>
       </c>
       <c r="C37" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>59</v>
       </c>
@@ -1325,10 +1364,13 @@
         <v>65</v>
       </c>
       <c r="C38" t="s">
+        <v>172</v>
+      </c>
+      <c r="D38" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -1336,10 +1378,13 @@
         <v>66</v>
       </c>
       <c r="C39" t="s">
+        <v>173</v>
+      </c>
+      <c r="D39" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -1350,7 +1395,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>67</v>
       </c>
@@ -1361,7 +1406,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>67</v>
       </c>
@@ -1372,7 +1417,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -1383,7 +1428,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -1394,7 +1439,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>67</v>
       </c>
@@ -1405,7 +1450,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>67</v>
       </c>
@@ -1416,7 +1461,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -1427,7 +1472,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -1438,7 +1483,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -1449,7 +1494,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -1460,7 +1505,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -1471,7 +1516,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -1482,7 +1527,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>82</v>
       </c>
@@ -1493,7 +1538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>82</v>
       </c>
@@ -1504,7 +1549,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -1515,7 +1560,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -1526,7 +1571,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -1537,7 +1582,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -1548,7 +1593,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>89</v>
       </c>
@@ -1559,7 +1604,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>89</v>
       </c>
@@ -1567,10 +1612,13 @@
         <v>92</v>
       </c>
       <c r="C60" t="s">
+        <v>174</v>
+      </c>
+      <c r="D60" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>89</v>
       </c>
@@ -1581,7 +1629,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>89</v>
       </c>
@@ -1592,7 +1640,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>89</v>
       </c>
@@ -1603,7 +1651,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>89</v>
       </c>

</xml_diff>